<commit_message>
Some updates and new Excel file data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/batch16ExcelFile.xlsx
+++ b/src/test/resources/testdata/batch16ExcelFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magre\IdeaProjects\HRMSB16\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0140EC-D20D-4825-9ABD-9E514B123D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF808D78-340F-4F00-8836-8A6E5AF3879B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="EmployeeDataBatch16" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -91,13 +90,13 @@
     <t>Abbel</t>
   </si>
   <si>
-    <t>best789</t>
-  </si>
-  <si>
-    <t>oldest456</t>
-  </si>
-  <si>
-    <t>fastest123</t>
+    <t>fire147</t>
+  </si>
+  <si>
+    <t>water258</t>
+  </si>
+  <si>
+    <t>soil369</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated ChromeDriver for headless run
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/batch16ExcelFile.xlsx
+++ b/src/test/resources/testdata/batch16ExcelFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magre\IdeaProjects\HRMSB16\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF808D78-340F-4F00-8836-8A6E5AF3879B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E77E22-61E7-4297-90A9-C75B54881D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,13 +90,13 @@
     <t>Abbel</t>
   </si>
   <si>
-    <t>fire147</t>
-  </si>
-  <si>
-    <t>water258</t>
-  </si>
-  <si>
     <t>soil369</t>
+  </si>
+  <si>
+    <t>fire963</t>
+  </si>
+  <si>
+    <t>water159</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -517,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -540,7 +540,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Updated data files for jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/batch16ExcelFile.xlsx
+++ b/src/test/resources/testdata/batch16ExcelFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magre\IdeaProjects\HRMSB16\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E77E22-61E7-4297-90A9-C75B54881D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FA1AE7-3BCE-4297-82AC-3FBB2A2F445E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,13 +90,13 @@
     <t>Abbel</t>
   </si>
   <si>
-    <t>soil369</t>
-  </si>
-  <si>
-    <t>fire963</t>
-  </si>
-  <si>
-    <t>water159</t>
+    <t>cold789</t>
+  </si>
+  <si>
+    <t>hot8945</t>
+  </si>
+  <si>
+    <t>worm357</t>
   </si>
 </sst>
 </file>
@@ -443,7 +443,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -494,7 +494,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -517,7 +517,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -540,7 +540,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Updated Excel file with dynamic username entries which will be removed in the end od testcase.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/batch16ExcelFile.xlsx
+++ b/src/test/resources/testdata/batch16ExcelFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magre\IdeaProjects\HRMSB16\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AFACAC-60C9-4A6F-A503-301A03DBFCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DEA04A-4FC5-41EC-BACE-8EAA73CD2BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="-11985" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployeeDataBatch16" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>firstName</t>
   </si>
@@ -78,13 +78,10 @@
     <t>Dan</t>
   </si>
   <si>
-    <t>vanelly17</t>
-  </si>
-  <si>
-    <t>vanelly27</t>
-  </si>
-  <si>
-    <t>vanelly37</t>
+    <t>1batch16id</t>
+  </si>
+  <si>
+    <t>Tim</t>
   </si>
 </sst>
 </file>
@@ -419,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -496,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
@@ -519,12 +516,35 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -534,8 +554,8 @@
     <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="F3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="G3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>